<commit_message>
Update related to Microsoft Store submission
</commit_message>
<xml_diff>
--- a/docs/List_of_Test_Cases.xlsx
+++ b/docs/List_of_Test_Cases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S.Sugawara\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S.Sugawara\GitHub\PathList\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EF40B3-1EC9-4EA1-9B9A-BE303BFC7960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26AD38E5-46E2-4EEB-B7B3-A480491F0969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A6278190-13FA-454D-85E9-C6F4CCBF8348}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="164">
   <si>
     <t>List</t>
     <phoneticPr fontId="1"/>
@@ -1342,13 +1342,7 @@
     <t>Font is 1 point larger than OS default</t>
   </si>
   <si>
-    <t>Main dialog and message</t>
-  </si>
-  <si>
     <t>Displayed in the center and foreground of the screen</t>
-  </si>
-  <si>
-    <t>Guidance indicating folders should be dropped is shown</t>
   </si>
   <si>
     <t>UI changes based on path list or tree structure selection</t>
@@ -1464,63 +1458,6 @@
       </rPr>
       <t>✓</t>
     </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>フォルダをドロップするべき案内が表示されること</t>
-    </r>
-    <rPh sb="13" eb="15">
-      <t>アンナイ</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>複数のフォルダがリスト化されること</t>
-    </r>
-    <rPh sb="0" eb="2">
-      <t>フクスウ</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>カ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>ショートカット先のフォルダがリスト化されること</t>
-    </r>
-    <rPh sb="7" eb="8">
-      <t>サキ</t>
-    </rPh>
-    <rPh sb="17" eb="18">
-      <t>カ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1633,6 +1570,148 @@
   </si>
   <si>
     <t>Output matches selected type (extension removed from filename)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>単独フォルダのドロップ</t>
+    <rPh sb="0" eb="2">
+      <t>タンドク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>単独ファイルのドロップ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>複数フォルダの同時ドロップ</t>
+    <rPh sb="0" eb="2">
+      <t>フクスウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ドウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>複数ファイルの同時ドロップ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Single folder drag-and-drop</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Multiple folder drag-and-drop</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Single file drag-and-drop</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Multiple file drag-and-drop</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>複数のフォルダがリスト化されること</t>
+    <rPh sb="0" eb="2">
+      <t>フクスウ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>カ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>同一フォルダが重複してリスト化されないこと</t>
+    <rPh sb="0" eb="2">
+      <t>ドウイツ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>チョウフク</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>バ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>No duplicate listing of the same folder</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>パスの未取得 / 取得済の表示</t>
+    <rPh sb="3" eb="6">
+      <t>ミシュトク</t>
+    </rPh>
+    <rPh sb="9" eb="12">
+      <t>シュトクスミ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>パス取得済時における再取得メッセージの表示</t>
+    <rPh sb="2" eb="5">
+      <t>シュトクズ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ジ</t>
+    </rPh>
+    <rPh sb="10" eb="13">
+      <t>サイシュトク</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>再取得メッセージが表示されること</t>
+    <rPh sb="0" eb="3">
+      <t>サイシュトク</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>フォルダ・ファイルドロップ時にダイアログの表示が更新されること</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The dialog display must be updated when a folder or file is dropped.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>A re‑retrieval message must be shown.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Show re‑retrieval message when path already retrieved</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Path status messages: prompt to drop / confirmation of retrieval</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メインダイアログが表示されること</t>
+    <rPh sb="9" eb="11">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>At Main dialog and messages</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The main dialog is displayed</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1851,7 +1930,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1968,6 +2047,33 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2428,20 +2534,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EAC72E-61CF-4F61-9868-481DC61A4854}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N62"/>
+  <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="18" customHeight="1" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="18" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="5" width="10.7109375" style="1"/>
-    <col min="6" max="6" width="60.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="70.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="70.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="70.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="60.7109375" style="1" customWidth="1"/>
+    <col min="7" max="9" width="70.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" style="1"/>
     <col min="11" max="11" width="10.7109375" style="27" customWidth="1"/>
     <col min="12" max="12" width="12.7109375" style="27" customWidth="1"/>
@@ -2461,7 +2565,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E1" s="15"/>
       <c r="F1" s="2" t="s">
@@ -2480,11 +2584,11 @@
         <v>3</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L1" s="15"/>
       <c r="M1" s="15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="N1" s="15"/>
     </row>
@@ -2526,12 +2630,12 @@
     </row>
     <row r="3" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>19</v>
@@ -2553,13 +2657,13 @@
         <v>1</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L3" s="23">
         <v>45936</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N3" s="23">
         <v>45936</v>
@@ -2579,7 +2683,7 @@
         <v>43</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H4" s="13" t="s">
         <v>44</v>
@@ -2588,17 +2692,17 @@
         <v>101</v>
       </c>
       <c r="J4" s="14">
-        <f t="shared" ref="J4:J62" si="0">ROW()-2</f>
+        <f t="shared" ref="J4:J65" si="0">ROW()-2</f>
         <v>2</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L4" s="24">
         <v>45936</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N4" s="24">
         <v>45936</v>
@@ -2624,20 +2728,20 @@
         <v>46</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>102</v>
+        <v>162</v>
       </c>
       <c r="J5" s="14">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L5" s="24">
         <v>45936</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N5" s="24">
         <v>45936</v>
@@ -2663,20 +2767,20 @@
         <v>48</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J6" s="14">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L6" s="24">
         <v>45936</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N6" s="24">
         <v>45936</v>
@@ -2698,27 +2802,27 @@
       <c r="G7" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="H7" s="17" t="s">
-        <v>136</v>
+      <c r="H7" s="42" t="s">
+        <v>161</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>104</v>
+        <v>163</v>
       </c>
       <c r="J7" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L7" s="25">
-        <v>45936</v>
+        <v>45985</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N7" s="25">
-        <v>45936</v>
+        <v>45985</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -2741,7 +2845,7 @@
         <v>51</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J8" s="18">
         <f t="shared" si="0"/>
@@ -2754,7 +2858,7 @@
         <v>4</v>
       </c>
       <c r="M8" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N8" s="25">
         <v>45936</v>
@@ -2762,7 +2866,7 @@
     </row>
     <row r="9" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>10</v>
@@ -2776,11 +2880,11 @@
       <c r="E9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>27</v>
+      <c r="F9" s="39" t="s">
+        <v>142</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>83</v>
+        <v>146</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
@@ -2789,13 +2893,13 @@
         <v>7</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L9" s="23">
         <v>45948</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N9" s="23">
         <v>45948</v>
@@ -2813,30 +2917,30 @@
       <c r="E10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>28</v>
+      <c r="F10" s="41" t="s">
+        <v>144</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>137</v>
+        <v>147</v>
+      </c>
+      <c r="H10" s="38" t="s">
+        <v>150</v>
       </c>
       <c r="I10" s="34" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J10" s="14">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L10" s="24">
         <v>45948</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N10" s="24">
         <v>45948</v>
@@ -2852,31 +2956,29 @@
       <c r="E11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="I11" s="13"/>
+      <c r="F11" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
       <c r="J11" s="14">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="L11" s="24">
-        <v>45948</v>
-      </c>
-      <c r="M11" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="N11" s="24">
-        <v>45948</v>
+        <v>124</v>
+      </c>
+      <c r="L11" s="45">
+        <v>45985</v>
+      </c>
+      <c r="M11" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="N11" s="45">
+        <v>45985</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -2889,29 +2991,33 @@
       <c r="E12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
+      <c r="F12" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="H12" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>152</v>
+      </c>
       <c r="J12" s="14">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="L12" s="24">
-        <v>45948</v>
-      </c>
-      <c r="M12" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="N12" s="24">
-        <v>45948</v>
+        <v>124</v>
+      </c>
+      <c r="L12" s="45">
+        <v>45985</v>
+      </c>
+      <c r="M12" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="N12" s="45">
+        <v>45985</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -2924,33 +3030,33 @@
       <c r="E13" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>38</v>
+      <c r="F13" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="H13" s="43" t="s">
+        <v>156</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>87</v>
+        <v>157</v>
       </c>
       <c r="J13" s="14">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="L13" s="24">
-        <v>45948</v>
-      </c>
-      <c r="M13" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="N13" s="24">
-        <v>45948</v>
+        <v>124</v>
+      </c>
+      <c r="L13" s="47">
+        <v>45985</v>
+      </c>
+      <c r="M13" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="N13" s="47">
+        <v>45985</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -2963,29 +3069,33 @@
       <c r="E14" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="13" t="s">
-        <v>39</v>
+      <c r="F14" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="G14" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="H14" s="38" t="s">
+        <v>155</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>88</v>
+        <v>158</v>
       </c>
       <c r="J14" s="14">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="L14" s="24">
-        <v>45948</v>
-      </c>
-      <c r="M14" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="N14" s="24">
-        <v>45948</v>
+        <v>124</v>
+      </c>
+      <c r="L14" s="47">
+        <v>45985</v>
+      </c>
+      <c r="M14" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="N14" s="47">
+        <v>45985</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -2993,34 +3103,34 @@
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="12" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>89</v>
-      </c>
+      <c r="F15" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
       <c r="J15" s="14">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="L15" s="24" t="s">
-        <v>4</v>
+        <v>123</v>
+      </c>
+      <c r="L15" s="24">
+        <v>45948</v>
       </c>
       <c r="M15" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N15" s="24">
-        <v>45949</v>
+        <v>45948</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -3028,34 +3138,38 @@
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="12" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
+      <c r="F16" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>131</v>
+      </c>
       <c r="H16" s="13" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J16" s="14">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="L16" s="24" t="s">
-        <v>4</v>
+        <v>123</v>
+      </c>
+      <c r="L16" s="24">
+        <v>45948</v>
       </c>
       <c r="M16" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N16" s="24">
-        <v>45949</v>
+        <v>45948</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -3063,7 +3177,7 @@
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="12" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>19</v>
@@ -3071,26 +3185,26 @@
       <c r="F17" s="20"/>
       <c r="G17" s="20"/>
       <c r="H17" s="13" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J17" s="14">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="L17" s="24" t="s">
-        <v>4</v>
+        <v>123</v>
+      </c>
+      <c r="L17" s="24">
+        <v>45948</v>
       </c>
       <c r="M17" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N17" s="24">
-        <v>45949</v>
+        <v>45948</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -3106,10 +3220,10 @@
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
       <c r="H18" s="13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J18" s="14">
         <f t="shared" si="0"/>
@@ -3122,7 +3236,7 @@
         <v>4</v>
       </c>
       <c r="M18" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N18" s="24">
         <v>45949</v>
@@ -3140,11 +3254,11 @@
       </c>
       <c r="F19" s="20"/>
       <c r="G19" s="20"/>
-      <c r="H19" s="38" t="s">
-        <v>145</v>
+      <c r="H19" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>146</v>
+        <v>90</v>
       </c>
       <c r="J19" s="14">
         <f t="shared" si="0"/>
@@ -3157,7 +3271,7 @@
         <v>4</v>
       </c>
       <c r="M19" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N19" s="24">
         <v>45949</v>
@@ -3176,10 +3290,10 @@
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
       <c r="H20" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J20" s="14">
         <f t="shared" si="0"/>
@@ -3192,7 +3306,7 @@
         <v>4</v>
       </c>
       <c r="M20" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N20" s="24">
         <v>45949</v>
@@ -3203,34 +3317,34 @@
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="12" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>92</v>
+      </c>
       <c r="J21" s="14">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="L21" s="24">
-        <v>45948</v>
+        <v>4</v>
+      </c>
+      <c r="L21" s="24" t="s">
+        <v>4</v>
       </c>
       <c r="M21" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N21" s="24">
-        <v>45948</v>
+        <v>45949</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -3243,17 +3357,13 @@
       <c r="E22" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="H22" s="13" t="s">
-        <v>58</v>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="38" t="s">
+        <v>140</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
       <c r="J22" s="14">
         <f t="shared" si="0"/>
@@ -3266,10 +3376,10 @@
         <v>4</v>
       </c>
       <c r="M22" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N22" s="24">
-        <v>45948</v>
+        <v>45949</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -3282,17 +3392,13 @@
       <c r="E23" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>96</v>
-      </c>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
       <c r="H23" s="13" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="J23" s="14">
         <f t="shared" si="0"/>
@@ -3305,46 +3411,42 @@
         <v>4</v>
       </c>
       <c r="M23" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N23" s="24">
-        <v>45948</v>
+        <v>45949</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
-      <c r="D24" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="H24" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="I24" s="13" t="s">
-        <v>108</v>
-      </c>
+      <c r="D24" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
       <c r="J24" s="14">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="L24" s="24" t="s">
-        <v>4</v>
+        <v>123</v>
+      </c>
+      <c r="L24" s="24">
+        <v>45948</v>
       </c>
       <c r="M24" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N24" s="24">
         <v>45948</v>
@@ -3354,30 +3456,38 @@
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="I25" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="J25" s="18">
+      <c r="D25" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="J25" s="14">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="K25" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="L25" s="25" t="s">
+      <c r="K25" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L25" s="24" t="s">
         <v>4</v>
       </c>
       <c r="M25" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="N25" s="25">
+        <v>123</v>
+      </c>
+      <c r="N25" s="24">
         <v>45948</v>
       </c>
     </row>
@@ -3385,46 +3495,62 @@
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="I26" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="J26" s="18">
+      <c r="D26" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="J26" s="14">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="K26" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="L26" s="25" t="s">
+      <c r="K26" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L26" s="24" t="s">
         <v>4</v>
       </c>
       <c r="M26" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="N26" s="25">
-        <v>45950</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="18" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+        <v>123</v>
+      </c>
+      <c r="N26" s="24">
+        <v>45948</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
+      <c r="D27" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>130</v>
+      </c>
       <c r="H27" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="J27" s="14">
         <f t="shared" si="0"/>
@@ -3437,110 +3563,92 @@
         <v>4</v>
       </c>
       <c r="M27" s="12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="N27" s="24">
         <v>45948</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="18" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
-      <c r="D28" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="F28" s="35" t="s">
-        <v>141</v>
-      </c>
-      <c r="G28" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="H28" s="37" t="s">
-        <v>142</v>
-      </c>
-      <c r="I28" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="J28" s="29">
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="I28" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="J28" s="18">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="K28" s="19"/>
-      <c r="L28" s="30"/>
-      <c r="M28" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="N28" s="30">
-        <v>45949</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="18" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="K28" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="L28" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="M28" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="N28" s="25">
+        <v>45948</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
-      <c r="C29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="10" t="s">
+      <c r="C29" s="8"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="I29" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="J29" s="18">
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="G29" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="11">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="K29" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="L29" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="M29" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="N29" s="23">
-        <v>45948</v>
+      <c r="K29" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="L29" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="M29" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="N29" s="25">
+        <v>45950</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="18" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
-      <c r="D30" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F30" s="13" t="s">
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="J30" s="14">
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="G30" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="I30" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="J30" s="14">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
       <c r="K30" s="12" t="s">
         <v>4</v>
       </c>
@@ -3548,7 +3656,7 @@
         <v>4</v>
       </c>
       <c r="M30" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N30" s="24">
         <v>45948</v>
@@ -3558,73 +3666,71 @@
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
-      <c r="D31" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="I31" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="J31" s="14">
+      <c r="D31" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="F31" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="H31" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="I31" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="J31" s="29">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="K31" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="L31" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M31" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="N31" s="24">
-        <v>45948</v>
+      <c r="K31" s="19"/>
+      <c r="L31" s="30"/>
+      <c r="M31" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="N31" s="30">
+        <v>45949</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="18" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="14">
+      <c r="C32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="11">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="K32" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="L32" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M32" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="N32" s="24">
+      <c r="K32" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="L32" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M32" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="N32" s="23">
         <v>45948</v>
       </c>
     </row>
@@ -3639,16 +3745,16 @@
         <v>19</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J33" s="14">
         <f t="shared" si="0"/>
@@ -3661,7 +3767,7 @@
         <v>4</v>
       </c>
       <c r="M33" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N33" s="24">
         <v>45948</v>
@@ -3678,16 +3784,16 @@
         <v>19</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I34" s="13" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J34" s="14">
         <f t="shared" si="0"/>
@@ -3700,7 +3806,7 @@
         <v>4</v>
       </c>
       <c r="M34" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N34" s="24">
         <v>45948</v>
@@ -3717,17 +3823,13 @@
         <v>19</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="H35" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="I35" s="13" t="s">
-        <v>115</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
       <c r="J35" s="14">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -3739,7 +3841,7 @@
         <v>4</v>
       </c>
       <c r="M35" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N35" s="24">
         <v>45948</v>
@@ -3748,75 +3850,79 @@
     <row r="36" spans="1:14" ht="18" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E36" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F36" s="35" t="s">
-        <v>141</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="H36" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="I36" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="J36" s="31">
+      <c r="C36" s="8"/>
+      <c r="D36" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="J36" s="14">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="K36" s="21"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="N36" s="32">
-        <v>45949</v>
+      <c r="K36" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L36" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="M36" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="N36" s="24">
+        <v>45948</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="18" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A37" s="8"/>
-      <c r="B37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="11">
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="J37" s="14">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="K37" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="L37" s="23">
-        <v>45936</v>
-      </c>
-      <c r="M37" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="N37" s="23">
-        <v>45936</v>
+      <c r="K37" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L37" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="M37" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="N37" s="24">
+        <v>45948</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="18" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
@@ -3824,103 +3930,111 @@
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
       <c r="D38" s="12" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E38" s="12" t="s">
         <v>19</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
+        <v>99</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>113</v>
+      </c>
       <c r="J38" s="14">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="K38" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="L38" s="24">
-        <v>45936</v>
+        <v>4</v>
+      </c>
+      <c r="L38" s="24" t="s">
+        <v>4</v>
       </c>
       <c r="M38" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N38" s="24">
-        <v>45936</v>
+        <v>45948</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="18" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F39" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="G39" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="14">
+      <c r="C39" s="3"/>
+      <c r="D39" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="G39" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="H39" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="I39" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="J39" s="31">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="K39" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="L39" s="24">
-        <v>45936</v>
-      </c>
-      <c r="M39" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="N39" s="24">
-        <v>45936</v>
+      <c r="K39" s="21"/>
+      <c r="L39" s="32"/>
+      <c r="M39" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="N39" s="32">
+        <v>45949</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="18" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F40" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G40" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="14">
+      <c r="B40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="11">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="K40" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="L40" s="24">
+      <c r="K40" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="L40" s="23">
         <v>45936</v>
       </c>
-      <c r="M40" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="N40" s="24">
+      <c r="M40" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="N40" s="23">
         <v>45936</v>
       </c>
     </row>
@@ -3935,10 +4049,10 @@
         <v>19</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H41" s="13"/>
       <c r="I41" s="13"/>
@@ -3947,13 +4061,13 @@
         <v>39</v>
       </c>
       <c r="K41" s="12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="L41" s="24">
         <v>45936</v>
       </c>
       <c r="M41" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N41" s="24">
         <v>45936</v>
@@ -3970,29 +4084,25 @@
         <v>19</v>
       </c>
       <c r="F42" s="13" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="H42" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="I42" s="13" t="s">
-        <v>117</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
       <c r="J42" s="14">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="K42" s="28" t="s">
-        <v>126</v>
+      <c r="K42" s="12" t="s">
+        <v>123</v>
       </c>
       <c r="L42" s="24">
         <v>45936</v>
       </c>
       <c r="M42" s="12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="N42" s="24">
         <v>45936</v>
@@ -4009,29 +4119,25 @@
         <v>19</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="H43" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="I43" s="13" t="s">
-        <v>118</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
       <c r="J43" s="14">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="K43" s="28" t="s">
-        <v>126</v>
+      <c r="K43" s="12" t="s">
+        <v>123</v>
       </c>
       <c r="L43" s="24">
         <v>45936</v>
       </c>
       <c r="M43" s="12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="N43" s="24">
         <v>45936</v>
@@ -4048,29 +4154,25 @@
         <v>19</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="H44" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I44" s="13" t="s">
-        <v>119</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
       <c r="J44" s="14">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="K44" s="28" t="s">
-        <v>126</v>
+      <c r="K44" s="12" t="s">
+        <v>124</v>
       </c>
       <c r="L44" s="24">
         <v>45936</v>
       </c>
       <c r="M44" s="12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="N44" s="24">
         <v>45936</v>
@@ -4079,7 +4181,7 @@
     <row r="45" spans="1:14" ht="18" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
-      <c r="C45" s="3"/>
+      <c r="C45" s="8"/>
       <c r="D45" s="12" t="s">
         <v>19</v>
       </c>
@@ -4087,29 +4189,29 @@
         <v>19</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I45" s="13" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="J45" s="14">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="K45" s="28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L45" s="24">
         <v>45936</v>
       </c>
       <c r="M45" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N45" s="24">
         <v>45936</v>
@@ -4118,37 +4220,39 @@
     <row r="46" spans="1:14" ht="18" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
-      <c r="C46" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G46" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H46" s="10"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="11">
+      <c r="C46" s="8"/>
+      <c r="D46" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G46" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="J46" s="14">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="K46" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="L46" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="M46" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="N46" s="23">
+      <c r="K46" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="L46" s="24">
+        <v>45936</v>
+      </c>
+      <c r="M46" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="N46" s="24">
         <v>45936</v>
       </c>
     </row>
@@ -4157,31 +4261,35 @@
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
       <c r="D47" s="12" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="E47" s="12" t="s">
         <v>19</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
+        <v>78</v>
+      </c>
+      <c r="H47" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>117</v>
+      </c>
       <c r="J47" s="14">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="K47" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="L47" s="24" t="s">
-        <v>4</v>
+      <c r="K47" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="L47" s="24">
+        <v>45936</v>
       </c>
       <c r="M47" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N47" s="24">
         <v>45936</v>
@@ -4190,33 +4298,37 @@
     <row r="48" spans="1:14" ht="18" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
+      <c r="C48" s="3"/>
       <c r="D48" s="12" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="E48" s="12" t="s">
         <v>19</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H48" s="13"/>
-      <c r="I48" s="13"/>
+        <v>79</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I48" s="13" t="s">
+        <v>118</v>
+      </c>
       <c r="J48" s="14">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="K48" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="L48" s="24" t="s">
-        <v>4</v>
+      <c r="K48" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="L48" s="24">
+        <v>45936</v>
       </c>
       <c r="M48" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N48" s="24">
         <v>45936</v>
@@ -4225,35 +4337,37 @@
     <row r="49" spans="1:14" ht="18" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E49" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F49" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G49" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
-      <c r="J49" s="14">
+      <c r="C49" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="11">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="K49" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="L49" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M49" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="N49" s="24">
+      <c r="K49" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="L49" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M49" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="N49" s="23">
         <v>45936</v>
       </c>
     </row>
@@ -4268,10 +4382,10 @@
         <v>19</v>
       </c>
       <c r="F50" s="13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G50" s="13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
@@ -4286,7 +4400,7 @@
         <v>4</v>
       </c>
       <c r="M50" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N50" s="24">
         <v>45936</v>
@@ -4303,17 +4417,13 @@
         <v>19</v>
       </c>
       <c r="F51" s="13" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="G51" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="H51" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="I51" s="13" t="s">
-        <v>117</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
       <c r="J51" s="14">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -4325,7 +4435,7 @@
         <v>4</v>
       </c>
       <c r="M51" s="12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="N51" s="24">
         <v>45936</v>
@@ -4342,17 +4452,13 @@
         <v>19</v>
       </c>
       <c r="F52" s="13" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="G52" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="H52" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="I52" s="13" t="s">
-        <v>118</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
       <c r="J52" s="14">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -4364,7 +4470,7 @@
         <v>4</v>
       </c>
       <c r="M52" s="12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="N52" s="24">
         <v>45936</v>
@@ -4374,24 +4480,20 @@
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
-      <c r="D53" s="16" t="s">
+      <c r="D53" s="12" t="s">
         <v>4</v>
       </c>
       <c r="E53" s="12" t="s">
         <v>19</v>
       </c>
       <c r="F53" s="13" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="G53" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="H53" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I53" s="13" t="s">
-        <v>119</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
       <c r="J53" s="14">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -4403,7 +4505,7 @@
         <v>4</v>
       </c>
       <c r="M53" s="12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="N53" s="24">
         <v>45936</v>
@@ -4413,23 +4515,23 @@
       <c r="A54" s="8"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
-      <c r="D54" s="16" t="s">
+      <c r="D54" s="12" t="s">
         <v>4</v>
       </c>
       <c r="E54" s="12" t="s">
         <v>19</v>
       </c>
       <c r="F54" s="13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H54" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I54" s="13" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="J54" s="14">
         <f t="shared" si="0"/>
@@ -4442,196 +4544,182 @@
         <v>4</v>
       </c>
       <c r="M54" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N54" s="24">
         <v>45936</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="18" customHeight="1" collapsed="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B55" s="2" t="s">
+    <row r="55" spans="1:14" ht="18" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G55" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H55" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I55" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="J55" s="14">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="K55" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L55" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="M55" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="N55" s="24">
+        <v>45936</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="18" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="8"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F56" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G56" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="H56" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I56" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="J56" s="14">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="K56" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L56" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="M56" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="N56" s="24">
+        <v>45936</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="18" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="8"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F57" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="G57" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="H57" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I57" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="J57" s="14">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="K57" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L57" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="M57" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="N57" s="24">
+        <v>45936</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="18" customHeight="1" collapsed="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C58" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D55" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G55" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H55" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I55" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J55" s="7">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="K55" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="L55" s="26">
-        <v>45936</v>
-      </c>
-      <c r="M55" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="N55" s="26">
-        <v>45936</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="8"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="4" t="s">
+      <c r="D58" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H58" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I58" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J58" s="7">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="K58" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="L58" s="26">
+        <v>45985</v>
+      </c>
+      <c r="M58" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="N58" s="26">
+        <v>45985</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="8"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D56" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H56" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I56" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J56" s="7">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="K56" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L56" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="M56" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="N56" s="26">
-        <v>45936</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="8"/>
-      <c r="B57" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H57" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I57" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J57" s="7">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="K57" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="L57" s="26">
-        <v>45950</v>
-      </c>
-      <c r="M57" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="N57" s="26">
-        <v>45950</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H58" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I58" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J58" s="7">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="K58" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L58" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="M58" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="N58" s="26">
-        <v>45950</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>0</v>
-      </c>
       <c r="D59" s="5" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>19</v>
@@ -4653,143 +4741,274 @@
         <v>57</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="L59" s="26">
-        <v>45936</v>
+        <v>4</v>
+      </c>
+      <c r="L59" s="26" t="s">
+        <v>4</v>
       </c>
       <c r="M59" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N59" s="26">
-        <v>45936</v>
+        <v>45985</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="8"/>
-      <c r="B60" s="3"/>
+      <c r="B60" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="C60" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J60" s="7">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="K60" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="L60" s="26">
+        <v>45985</v>
+      </c>
+      <c r="M60" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="N60" s="26">
+        <v>45985</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D60" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G60" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H60" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I60" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J60" s="7">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="K60" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L60" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="M60" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="N60" s="26">
-        <v>45936</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="8"/>
-      <c r="B61" s="2" t="s">
+      <c r="D61" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H61" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I61" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J61" s="7">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="K61" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L61" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="M61" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="N61" s="26">
+        <v>45985</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H62" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I62" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J62" s="7">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="K62" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="L62" s="26">
+        <v>45985</v>
+      </c>
+      <c r="M62" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="N62" s="26">
+        <v>45985</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="8"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I63" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J63" s="7">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="K63" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L63" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="M63" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="N63" s="26">
+        <v>45985</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="8"/>
+      <c r="B64" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C64" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D61" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G61" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H61" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I61" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J61" s="7">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="K61" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="L61" s="26">
-        <v>45950</v>
-      </c>
-      <c r="M61" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="N61" s="26">
-        <v>45950</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3" t="s">
+      <c r="D64" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H64" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I64" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J64" s="7">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="K64" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="L64" s="26">
+        <v>45985</v>
+      </c>
+      <c r="M64" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="N64" s="26">
+        <v>45985</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C65" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D62" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G62" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H62" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I62" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J62" s="7">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="K62" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L62" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="M62" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="N62" s="26">
-        <v>45950</v>
+      <c r="D65" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I65" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J65" s="7">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="K65" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L65" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="M65" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="N65" s="26">
+        <v>45985</v>
       </c>
     </row>
   </sheetData>

</xml_diff>